<commit_message>
Further fixes in light of secondary template dataset
A fresh dataset has shown a number of issues that affect Scope 2 estimation as well as other latent issues (Oil and Gas sector, currency definitions and conversion, target date validation, canonical NaNs, etc).

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data/20220927 ITR Tool Test Data.xlsx
+++ b/examples/data/20220927 ITR Tool Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/MichaelTiemannOSC/ITR/examples/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68358E9B-BA50-B241-87F3-4966BBFE735C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC5319E-3191-8E4C-93C7-E41165A1EBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="77140" windowHeight="31860" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="43240" windowHeight="31860" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AT2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="AT6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU2" authorId="0" shapeId="0" xr:uid="{761CBD8A-501A-504B-AB1B-A55C5BB16672}">
+    <comment ref="AU6" authorId="0" shapeId="0" xr:uid="{761CBD8A-501A-504B-AB1B-A55C5BB16672}">
       <text>
         <r>
           <rPr>
@@ -99,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV2" authorId="0" shapeId="0" xr:uid="{87C76978-2E92-454C-9228-2A19D8E06C22}">
+    <comment ref="AV6" authorId="0" shapeId="0" xr:uid="{87C76978-2E92-454C-9228-2A19D8E06C22}">
       <text>
         <r>
           <rPr>
@@ -124,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW2" authorId="0" shapeId="0" xr:uid="{130DC316-804F-7541-9C87-4870EAF1A6F6}">
+    <comment ref="AW6" authorId="0" shapeId="0" xr:uid="{130DC316-804F-7541-9C87-4870EAF1A6F6}">
       <text>
         <r>
           <rPr>
@@ -149,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX2" authorId="0" shapeId="0" xr:uid="{E987B55C-EB00-FA4E-8CE1-71A118A0FF17}">
+    <comment ref="AX6" authorId="0" shapeId="0" xr:uid="{E987B55C-EB00-FA4E-8CE1-71A118A0FF17}">
       <text>
         <r>
           <rPr>
@@ -174,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT3" authorId="0" shapeId="0" xr:uid="{27FA3010-13C1-DC40-8B59-25A71AA35F05}">
+    <comment ref="AT7" authorId="0" shapeId="0" xr:uid="{27FA3010-13C1-DC40-8B59-25A71AA35F05}">
       <text>
         <r>
           <rPr>
@@ -199,7 +199,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU3" authorId="0" shapeId="0" xr:uid="{0B06AAB8-1777-DD40-ACE2-EDB803638737}">
+    <comment ref="AU7" authorId="0" shapeId="0" xr:uid="{0B06AAB8-1777-DD40-ACE2-EDB803638737}">
       <text>
         <r>
           <rPr>
@@ -224,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV3" authorId="0" shapeId="0" xr:uid="{801285E1-E2DF-1148-A716-99497AB21411}">
+    <comment ref="AV7" authorId="0" shapeId="0" xr:uid="{801285E1-E2DF-1148-A716-99497AB21411}">
       <text>
         <r>
           <rPr>
@@ -249,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW3" authorId="0" shapeId="0" xr:uid="{1E090C53-B6B1-FC49-B73F-C9DB47A48933}">
+    <comment ref="AW7" authorId="0" shapeId="0" xr:uid="{1E090C53-B6B1-FC49-B73F-C9DB47A48933}">
       <text>
         <r>
           <rPr>
@@ -274,7 +274,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX3" authorId="0" shapeId="0" xr:uid="{5CD86015-A9FB-2E48-B50F-B4796E1288E8}">
+    <comment ref="AX7" authorId="0" shapeId="0" xr:uid="{5CD86015-A9FB-2E48-B50F-B4796E1288E8}">
       <text>
         <r>
           <rPr>
@@ -299,7 +299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT4" authorId="0" shapeId="0" xr:uid="{10CE8AAD-83E4-3F48-A5D9-28FA677205F6}">
+    <comment ref="AT8" authorId="0" shapeId="0" xr:uid="{10CE8AAD-83E4-3F48-A5D9-28FA677205F6}">
       <text>
         <r>
           <rPr>
@@ -324,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU4" authorId="0" shapeId="0" xr:uid="{64282D69-0044-5D4F-85DF-D113CEFC5D26}">
+    <comment ref="AU8" authorId="0" shapeId="0" xr:uid="{64282D69-0044-5D4F-85DF-D113CEFC5D26}">
       <text>
         <r>
           <rPr>
@@ -349,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV4" authorId="0" shapeId="0" xr:uid="{4BE9897A-8852-6B40-895A-4AD9308CE01E}">
+    <comment ref="AV8" authorId="0" shapeId="0" xr:uid="{4BE9897A-8852-6B40-895A-4AD9308CE01E}">
       <text>
         <r>
           <rPr>
@@ -374,7 +374,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW4" authorId="0" shapeId="0" xr:uid="{53DE15ED-45AF-FE47-9615-70D775F21605}">
+    <comment ref="AW8" authorId="0" shapeId="0" xr:uid="{53DE15ED-45AF-FE47-9615-70D775F21605}">
       <text>
         <r>
           <rPr>
@@ -399,7 +399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX4" authorId="0" shapeId="0" xr:uid="{3AFC24B3-56D3-7241-A257-B01B8F429222}">
+    <comment ref="AX8" authorId="0" shapeId="0" xr:uid="{3AFC24B3-56D3-7241-A257-B01B8F429222}">
       <text>
         <r>
           <rPr>
@@ -424,7 +424,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT5" authorId="0" shapeId="0" xr:uid="{AD8E86C7-F029-8D42-B90D-191D1ED20F7C}">
+    <comment ref="AT9" authorId="0" shapeId="0" xr:uid="{AD8E86C7-F029-8D42-B90D-191D1ED20F7C}">
       <text>
         <r>
           <rPr>
@@ -449,7 +449,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU5" authorId="0" shapeId="0" xr:uid="{74C2EBCC-00E9-9043-BE45-46AD76BC81F5}">
+    <comment ref="AU9" authorId="0" shapeId="0" xr:uid="{74C2EBCC-00E9-9043-BE45-46AD76BC81F5}">
       <text>
         <r>
           <rPr>
@@ -474,7 +474,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV5" authorId="0" shapeId="0" xr:uid="{A56B5F82-82D3-AA4E-80C4-6AF728B5EAE4}">
+    <comment ref="AV9" authorId="0" shapeId="0" xr:uid="{A56B5F82-82D3-AA4E-80C4-6AF728B5EAE4}">
       <text>
         <r>
           <rPr>
@@ -499,7 +499,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW5" authorId="0" shapeId="0" xr:uid="{5A2CB172-2E17-304F-A551-840B5508588D}">
+    <comment ref="AW9" authorId="0" shapeId="0" xr:uid="{5A2CB172-2E17-304F-A551-840B5508588D}">
       <text>
         <r>
           <rPr>
@@ -524,7 +524,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX5" authorId="0" shapeId="0" xr:uid="{98E481A3-D51D-F942-AFCA-E0FFE101C3A8}">
+    <comment ref="AX9" authorId="0" shapeId="0" xr:uid="{98E481A3-D51D-F942-AFCA-E0FFE101C3A8}">
       <text>
         <r>
           <rPr>
@@ -1106,7 +1106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2204" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="407">
   <si>
     <t>company_name</t>
   </si>
@@ -2542,6 +2542,15 @@
   </si>
   <si>
     <t>investment_value [USD]</t>
+  </si>
+  <si>
+    <t>RWE AG</t>
+  </si>
+  <si>
+    <t>529900GB7KCA94ACC940</t>
+  </si>
+  <si>
+    <t>DE0007037129</t>
   </si>
 </sst>
 </file>
@@ -4273,11 +4282,11 @@
   </sheetPr>
   <dimension ref="A1:AZ11"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AE1" sqref="AE1"/>
       <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
-      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
+      <selection pane="bottomRight" activeCell="AZ2" sqref="AZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -4450,20 +4459,20 @@
     </row>
     <row r="2" spans="1:52">
       <c r="A2" t="s">
-        <v>388</v>
+        <v>404</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>405</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>406</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E2" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="E2"/>
       <c r="F2" t="s">
-        <v>399</v>
+        <v>55</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>56</v>
@@ -4475,154 +4484,155 @@
         <v>44561</v>
       </c>
       <c r="J2">
-        <v>16000</v>
+        <v>27350000000</v>
       </c>
       <c r="K2">
-        <v>2000</v>
+        <v>29017000000</v>
       </c>
       <c r="L2">
-        <v>100000</v>
+        <v>16000000000</v>
       </c>
       <c r="M2">
-        <v>400000</v>
+        <v>32404000000</v>
       </c>
       <c r="N2">
-        <f>1000000+L2</f>
-        <v>1100000</v>
+        <v>168366000000</v>
       </c>
       <c r="O2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="P2" t="s">
-        <v>402</v>
-      </c>
-      <c r="Q2">
-        <v>1000</v>
-      </c>
-      <c r="R2">
-        <v>995</v>
+        <v>65</v>
+      </c>
+      <c r="Q2" s="20">
+        <v>155.30000000000001</v>
+      </c>
+      <c r="R2" s="20">
+        <v>136.6</v>
       </c>
       <c r="S2">
-        <v>990</v>
+        <v>125.4</v>
       </c>
       <c r="T2">
-        <v>985</v>
+        <v>91.7</v>
       </c>
       <c r="U2">
-        <v>980</v>
+        <v>70.2</v>
       </c>
       <c r="V2">
-        <v>975</v>
-      </c>
-      <c r="W2"/>
+        <v>86.9</v>
+      </c>
+      <c r="W2" s="4">
+        <v>89.6</v>
+      </c>
       <c r="X2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>97</v>
+        <v>4.7</v>
       </c>
       <c r="AB2">
-        <v>96</v>
-      </c>
-      <c r="AC2">
-        <v>95</v>
-      </c>
-      <c r="AD2" s="18"/>
+        <v>3.1</v>
+      </c>
+      <c r="AC2" s="20">
+        <v>2.7</v>
+      </c>
+      <c r="AD2" s="4">
+        <v>2.8</v>
+      </c>
       <c r="AE2" s="19">
-        <f t="shared" ref="AE2:AK3" si="0">IF(ISBLANK(Q2),IF(ISBLANK(X2),"",X2),Q2+X2)</f>
-        <v>1100</v>
+        <f t="shared" ref="AE2" si="0">IF(ISBLANK(Q2),IF(ISBLANK(X2),"",X2),Q2+X2)</f>
+        <v>155.30000000000001</v>
       </c>
       <c r="AF2" s="19">
-        <f t="shared" si="0"/>
-        <v>1094</v>
+        <f t="shared" ref="AF2" si="1">IF(ISBLANK(R2),IF(ISBLANK(Y2),"",Y2),R2+Y2)</f>
+        <v>136.6</v>
       </c>
       <c r="AG2" s="19">
-        <f t="shared" si="0"/>
-        <v>1088</v>
+        <f t="shared" ref="AG2" si="2">IF(ISBLANK(S2),IF(ISBLANK(Z2),"",Z2),S2+Z2)</f>
+        <v>125.4</v>
       </c>
       <c r="AH2" s="19">
-        <f t="shared" si="0"/>
-        <v>1082</v>
+        <f t="shared" ref="AH2" si="3">IF(ISBLANK(T2),IF(ISBLANK(AA2),"",AA2),T2+AA2)</f>
+        <v>96.4</v>
       </c>
       <c r="AI2" s="19">
-        <f t="shared" si="0"/>
-        <v>1076</v>
+        <f t="shared" ref="AI2" si="4">IF(ISBLANK(U2),IF(ISBLANK(AB2),"",AB2),U2+AB2)</f>
+        <v>73.3</v>
       </c>
       <c r="AJ2" s="19">
-        <f t="shared" si="0"/>
-        <v>1070</v>
-      </c>
-      <c r="AK2" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="AL2" s="18">
+        <f t="shared" ref="AJ2" si="5">IF(ISBLANK(V2),IF(ISBLANK(AC2),"",AC2),V2+AC2)</f>
+        <v>89.600000000000009</v>
+      </c>
+      <c r="AK2" s="19">
+        <f t="shared" ref="AK2" si="6">IF(ISBLANK(W2),IF(ISBLANK(AD2),"",AD2),W2+AD2)</f>
+        <v>92.399999999999991</v>
+      </c>
+      <c r="AL2">
         <v>0</v>
       </c>
-      <c r="AM2" s="18">
+      <c r="AM2">
         <v>0</v>
       </c>
-      <c r="AN2" s="18">
+      <c r="AN2">
         <v>0</v>
       </c>
-      <c r="AO2" s="18">
+      <c r="AO2">
         <v>0</v>
       </c>
-      <c r="AP2" s="18">
+      <c r="AP2">
         <v>0</v>
       </c>
-      <c r="AQ2" s="18">
+      <c r="AQ2">
         <v>0</v>
       </c>
-      <c r="AR2" s="18"/>
-      <c r="AS2">
-        <v>3</v>
-      </c>
-      <c r="AT2">
-        <f>AS2+0.1</f>
-        <v>3.1</v>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="21">
+        <v>216</v>
+      </c>
+      <c r="AT2" s="21">
+        <v>200</v>
       </c>
       <c r="AU2">
-        <f t="shared" ref="AU2:AX2" si="1">AT2+0.1</f>
-        <v>3.2</v>
+        <v>176</v>
       </c>
       <c r="AV2">
-        <f t="shared" si="1"/>
-        <v>3.3000000000000003</v>
+        <v>153</v>
       </c>
       <c r="AW2">
-        <f t="shared" si="1"/>
-        <v>3.4000000000000004</v>
-      </c>
-      <c r="AX2">
-        <f t="shared" si="1"/>
-        <v>3.5000000000000004</v>
-      </c>
-      <c r="AY2" s="18"/>
-      <c r="AZ2" s="18"/>
+        <v>146.755</v>
+      </c>
+      <c r="AX2" s="20">
+        <v>166.56</v>
+      </c>
+      <c r="AY2">
+        <v>162.61199999999999</v>
+      </c>
     </row>
     <row r="3" spans="1:52">
       <c r="A3" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>393</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>54</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" t="s">
-        <v>399</v>
+        <v>55</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>56</v>
@@ -4633,152 +4643,140 @@
       <c r="I3" s="3">
         <v>44561</v>
       </c>
-      <c r="J3">
-        <v>8000</v>
-      </c>
-      <c r="K3">
-        <v>4000</v>
-      </c>
-      <c r="L3">
-        <v>200000</v>
-      </c>
-      <c r="M3">
-        <v>400000</v>
-      </c>
-      <c r="N3">
-        <f>1000000+L3</f>
-        <v>1200000</v>
+      <c r="J3" s="22">
+        <v>19310000000</v>
+      </c>
+      <c r="K3" s="22">
+        <v>6974000000</v>
+      </c>
+      <c r="L3" s="22">
+        <v>25930000000</v>
+      </c>
+      <c r="M3" s="22">
+        <f>L3+411000000</f>
+        <v>26341000000</v>
+      </c>
+      <c r="N3" s="22">
+        <v>39504000000</v>
       </c>
       <c r="O3" t="s">
         <v>58</v>
       </c>
       <c r="P3" t="s">
-        <v>402</v>
-      </c>
-      <c r="Q3">
-        <v>1000</v>
-      </c>
-      <c r="R3">
-        <v>995</v>
+        <v>59</v>
+      </c>
+      <c r="Q3" s="20">
+        <v>1040335</v>
+      </c>
+      <c r="R3" s="20">
+        <v>965570</v>
       </c>
       <c r="S3">
-        <v>990</v>
+        <v>1363231</v>
       </c>
       <c r="T3">
-        <v>985</v>
+        <v>1934393</v>
       </c>
       <c r="U3">
-        <v>980</v>
+        <v>1416448</v>
       </c>
       <c r="V3">
-        <v>975</v>
-      </c>
-      <c r="W3"/>
+        <f>1590305</f>
+        <v>1590305</v>
+      </c>
       <c r="X3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Y3">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="Z3">
-        <v>98</v>
+        <v>381533</v>
       </c>
       <c r="AA3">
-        <v>97</v>
+        <v>231192</v>
       </c>
       <c r="AB3">
-        <v>96</v>
-      </c>
-      <c r="AC3">
-        <v>95</v>
-      </c>
-      <c r="AD3"/>
+        <v>297283</v>
+      </c>
+      <c r="AC3" s="20">
+        <v>273432</v>
+      </c>
       <c r="AE3" s="19">
-        <f t="shared" si="0"/>
-        <v>1100</v>
+        <f t="shared" ref="AE3:AK4" si="7">IF(ISBLANK(Q3),IF(ISBLANK(X3),"",X3),Q3+X3)</f>
+        <v>1040335</v>
       </c>
       <c r="AF3" s="19">
-        <f t="shared" si="0"/>
-        <v>1094</v>
+        <f t="shared" ref="AF3" si="8">IF(ISBLANK(R3),IF(ISBLANK(Y3),"",Y3),R3+Y3)</f>
+        <v>965570</v>
       </c>
       <c r="AG3" s="19">
-        <f t="shared" si="0"/>
-        <v>1088</v>
+        <f t="shared" ref="AG3" si="9">IF(ISBLANK(S3),IF(ISBLANK(Z3),"",Z3),S3+Z3)</f>
+        <v>1744764</v>
       </c>
       <c r="AH3" s="19">
-        <f t="shared" si="0"/>
-        <v>1082</v>
+        <f t="shared" ref="AH3" si="10">IF(ISBLANK(T3),IF(ISBLANK(AA3),"",AA3),T3+AA3)</f>
+        <v>2165585</v>
       </c>
       <c r="AI3" s="19">
-        <f t="shared" si="0"/>
-        <v>1076</v>
+        <f t="shared" ref="AI3" si="11">IF(ISBLANK(U3),IF(ISBLANK(AB3),"",AB3),U3+AB3)</f>
+        <v>1713731</v>
       </c>
       <c r="AJ3" s="19">
-        <f t="shared" si="0"/>
-        <v>1070</v>
+        <f t="shared" ref="AJ3" si="12">IF(ISBLANK(V3),IF(ISBLANK(AC3),"",AC3),V3+AC3)</f>
+        <v>1863737</v>
       </c>
       <c r="AK3" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AK3" si="13">IF(ISBLANK(W3),IF(ISBLANK(AD3),"",AD3),W3+AD3)</f>
         <v/>
       </c>
-      <c r="AL3" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AM3" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AN3" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AO3" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AP3" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AQ3" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AS3">
-        <v>3</v>
-      </c>
-      <c r="AT3">
-        <f t="shared" ref="AT3:AX3" si="2">AS3+0.1</f>
-        <v>3.1</v>
+      <c r="AN3">
+        <v>21590220</v>
+      </c>
+      <c r="AO3">
+        <v>19892852</v>
+      </c>
+      <c r="AP3">
+        <v>24528246</v>
+      </c>
+      <c r="AQ3" s="20">
+        <v>21996103</v>
+      </c>
+      <c r="AS3" s="21">
+        <v>17912</v>
+      </c>
+      <c r="AT3" s="21">
+        <v>18104</v>
       </c>
       <c r="AU3">
-        <f t="shared" si="2"/>
-        <v>3.2</v>
+        <v>20057</v>
       </c>
       <c r="AV3">
-        <f t="shared" si="2"/>
-        <v>3.3000000000000003</v>
+        <v>20960</v>
       </c>
       <c r="AW3">
-        <f t="shared" si="2"/>
-        <v>3.4000000000000004</v>
-      </c>
-      <c r="AX3">
-        <f t="shared" si="2"/>
-        <v>3.5000000000000004</v>
+        <v>22142</v>
+      </c>
+      <c r="AX3" s="20">
+        <v>22591</v>
       </c>
     </row>
     <row r="4" spans="1:52">
       <c r="A4" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>395</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>54</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>56</v>
@@ -4789,148 +4787,136 @@
       <c r="I4" s="3">
         <v>44561</v>
       </c>
-      <c r="J4">
-        <v>4000</v>
-      </c>
-      <c r="K4">
-        <v>8000</v>
-      </c>
-      <c r="L4">
-        <v>300000</v>
-      </c>
-      <c r="M4">
-        <v>400000</v>
-      </c>
-      <c r="N4">
-        <f>1000000+L4</f>
-        <v>1300000</v>
+      <c r="J4" s="22">
+        <v>19310000000</v>
+      </c>
+      <c r="K4" s="22">
+        <v>6974000000</v>
+      </c>
+      <c r="L4" s="22">
+        <v>25930000000</v>
+      </c>
+      <c r="M4" s="22">
+        <f>L4+411000000</f>
+        <v>26341000000</v>
+      </c>
+      <c r="N4" s="22">
+        <v>39504000000</v>
       </c>
       <c r="O4" t="s">
         <v>58</v>
       </c>
       <c r="P4" t="s">
-        <v>402</v>
-      </c>
-      <c r="Q4">
-        <v>1000</v>
-      </c>
-      <c r="R4">
-        <v>995</v>
+        <v>59</v>
+      </c>
+      <c r="Q4" s="20">
+        <v>1040335</v>
+      </c>
+      <c r="R4" s="20">
+        <v>965570</v>
       </c>
       <c r="S4">
-        <v>990</v>
+        <v>1363231</v>
       </c>
       <c r="T4">
-        <v>985</v>
+        <v>1934393</v>
       </c>
       <c r="U4">
-        <v>980</v>
+        <v>1416448</v>
       </c>
       <c r="V4">
-        <v>975</v>
-      </c>
-      <c r="W4"/>
+        <f>1590305</f>
+        <v>1590305</v>
+      </c>
       <c r="X4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Y4">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="Z4">
-        <v>98</v>
+        <v>381533</v>
       </c>
       <c r="AA4">
-        <v>97</v>
+        <v>231192</v>
       </c>
       <c r="AB4">
-        <v>96</v>
-      </c>
-      <c r="AC4">
-        <v>95</v>
-      </c>
-      <c r="AD4"/>
+        <v>297283</v>
+      </c>
+      <c r="AC4" s="20">
+        <v>273432</v>
+      </c>
       <c r="AE4" s="19">
-        <f t="shared" ref="AE4" si="3">IF(ISBLANK(Q4),IF(ISBLANK(X4),"",X4),Q4+X4)</f>
-        <v>1100</v>
+        <f t="shared" si="7"/>
+        <v>1040335</v>
       </c>
       <c r="AF4" s="19">
-        <f t="shared" ref="AF4" si="4">IF(ISBLANK(R4),IF(ISBLANK(Y4),"",Y4),R4+Y4)</f>
-        <v>1094</v>
+        <f t="shared" si="7"/>
+        <v>965570</v>
       </c>
       <c r="AG4" s="19">
-        <f t="shared" ref="AG4" si="5">IF(ISBLANK(S4),IF(ISBLANK(Z4),"",Z4),S4+Z4)</f>
-        <v>1088</v>
+        <f t="shared" si="7"/>
+        <v>1744764</v>
       </c>
       <c r="AH4" s="19">
-        <f t="shared" ref="AH4" si="6">IF(ISBLANK(T4),IF(ISBLANK(AA4),"",AA4),T4+AA4)</f>
-        <v>1082</v>
+        <f t="shared" si="7"/>
+        <v>2165585</v>
       </c>
       <c r="AI4" s="19">
-        <f t="shared" ref="AI4" si="7">IF(ISBLANK(U4),IF(ISBLANK(AB4),"",AB4),U4+AB4)</f>
-        <v>1076</v>
+        <f t="shared" si="7"/>
+        <v>1713731</v>
       </c>
       <c r="AJ4" s="19">
-        <f t="shared" ref="AJ4" si="8">IF(ISBLANK(V4),IF(ISBLANK(AC4),"",AC4),V4+AC4)</f>
-        <v>1070</v>
+        <f t="shared" si="7"/>
+        <v>1863737</v>
       </c>
       <c r="AK4" s="19" t="str">
-        <f t="shared" ref="AK4" si="9">IF(ISBLANK(W4),IF(ISBLANK(AD4),"",AD4),W4+AD4)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="AL4" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AM4" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AN4" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AO4" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AP4" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AQ4" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AS4">
-        <v>3</v>
-      </c>
-      <c r="AT4">
-        <f t="shared" ref="AT4:AX4" si="10">AS4+0.1</f>
-        <v>3.1</v>
+      <c r="AN4">
+        <v>21590220</v>
+      </c>
+      <c r="AO4">
+        <v>19892852</v>
+      </c>
+      <c r="AP4">
+        <v>24528246</v>
+      </c>
+      <c r="AQ4" s="20">
+        <v>21996103</v>
+      </c>
+      <c r="AS4" s="21">
+        <v>17912</v>
+      </c>
+      <c r="AT4" s="21">
+        <v>18104</v>
       </c>
       <c r="AU4">
-        <f t="shared" si="10"/>
-        <v>3.2</v>
+        <v>20057</v>
       </c>
       <c r="AV4">
-        <f t="shared" si="10"/>
-        <v>3.3000000000000003</v>
+        <v>20960</v>
       </c>
       <c r="AW4">
-        <f t="shared" si="10"/>
-        <v>3.4000000000000004</v>
-      </c>
-      <c r="AX4">
-        <f t="shared" si="10"/>
-        <v>3.5000000000000004</v>
+        <v>22142</v>
+      </c>
+      <c r="AX4" s="20">
+        <v>22591</v>
       </c>
     </row>
     <row r="5" spans="1:52">
       <c r="A5" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>401</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>54</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" t="s">
@@ -4945,152 +4931,140 @@
       <c r="I5" s="3">
         <v>44561</v>
       </c>
-      <c r="J5">
-        <v>2000</v>
-      </c>
-      <c r="K5">
-        <v>16000</v>
-      </c>
-      <c r="L5">
-        <v>400000</v>
-      </c>
-      <c r="M5">
-        <v>400000</v>
-      </c>
-      <c r="N5">
-        <f>1000000+L5</f>
-        <v>1400000</v>
+      <c r="J5" s="22">
+        <v>19310000000</v>
+      </c>
+      <c r="K5" s="22">
+        <v>6974000000</v>
+      </c>
+      <c r="L5" s="22">
+        <v>25930000000</v>
+      </c>
+      <c r="M5" s="22">
+        <f>L5+411000000</f>
+        <v>26341000000</v>
+      </c>
+      <c r="N5" s="22">
+        <v>39504000000</v>
       </c>
       <c r="O5" t="s">
         <v>58</v>
       </c>
       <c r="P5" t="s">
-        <v>402</v>
-      </c>
-      <c r="Q5">
-        <v>1000</v>
-      </c>
-      <c r="R5">
-        <v>995</v>
+        <v>59</v>
+      </c>
+      <c r="Q5" s="20">
+        <v>1040335</v>
+      </c>
+      <c r="R5" s="20">
+        <v>965570</v>
       </c>
       <c r="S5">
-        <v>990</v>
+        <v>1363231</v>
       </c>
       <c r="T5">
-        <v>985</v>
+        <v>1934393</v>
       </c>
       <c r="U5">
-        <v>980</v>
+        <v>1416448</v>
       </c>
       <c r="V5">
-        <v>975</v>
-      </c>
-      <c r="W5"/>
+        <f>1590305</f>
+        <v>1590305</v>
+      </c>
       <c r="X5">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Y5">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="Z5">
-        <v>98</v>
+        <v>381533</v>
       </c>
       <c r="AA5">
-        <v>97</v>
+        <v>231192</v>
       </c>
       <c r="AB5">
-        <v>96</v>
-      </c>
-      <c r="AC5">
-        <v>95</v>
-      </c>
-      <c r="AD5"/>
+        <v>297283</v>
+      </c>
+      <c r="AC5" s="20">
+        <v>273432</v>
+      </c>
       <c r="AE5" s="19">
-        <f t="shared" ref="AE5:AK7" si="11">IF(ISBLANK(Q5),IF(ISBLANK(X5),"",X5),Q5+X5)</f>
-        <v>1100</v>
+        <f t="shared" ref="AE5" si="14">IF(ISBLANK(Q5),IF(ISBLANK(X5),"",X5),Q5+X5)</f>
+        <v>1040335</v>
       </c>
       <c r="AF5" s="19">
-        <f t="shared" ref="AF5:AF6" si="12">IF(ISBLANK(R5),IF(ISBLANK(Y5),"",Y5),R5+Y5)</f>
-        <v>1094</v>
+        <f t="shared" ref="AF5" si="15">IF(ISBLANK(R5),IF(ISBLANK(Y5),"",Y5),R5+Y5)</f>
+        <v>965570</v>
       </c>
       <c r="AG5" s="19">
-        <f t="shared" ref="AG5:AG6" si="13">IF(ISBLANK(S5),IF(ISBLANK(Z5),"",Z5),S5+Z5)</f>
-        <v>1088</v>
+        <f t="shared" ref="AG5" si="16">IF(ISBLANK(S5),IF(ISBLANK(Z5),"",Z5),S5+Z5)</f>
+        <v>1744764</v>
       </c>
       <c r="AH5" s="19">
-        <f t="shared" ref="AH5:AH6" si="14">IF(ISBLANK(T5),IF(ISBLANK(AA5),"",AA5),T5+AA5)</f>
-        <v>1082</v>
+        <f t="shared" ref="AH5" si="17">IF(ISBLANK(T5),IF(ISBLANK(AA5),"",AA5),T5+AA5)</f>
+        <v>2165585</v>
       </c>
       <c r="AI5" s="19">
-        <f t="shared" ref="AI5:AI6" si="15">IF(ISBLANK(U5),IF(ISBLANK(AB5),"",AB5),U5+AB5)</f>
-        <v>1076</v>
+        <f t="shared" ref="AI5" si="18">IF(ISBLANK(U5),IF(ISBLANK(AB5),"",AB5),U5+AB5)</f>
+        <v>1713731</v>
       </c>
       <c r="AJ5" s="19">
-        <f t="shared" ref="AJ5:AJ6" si="16">IF(ISBLANK(V5),IF(ISBLANK(AC5),"",AC5),V5+AC5)</f>
-        <v>1070</v>
+        <f t="shared" ref="AJ5" si="19">IF(ISBLANK(V5),IF(ISBLANK(AC5),"",AC5),V5+AC5)</f>
+        <v>1863737</v>
       </c>
       <c r="AK5" s="19" t="str">
-        <f t="shared" ref="AK5:AK6" si="17">IF(ISBLANK(W5),IF(ISBLANK(AD5),"",AD5),W5+AD5)</f>
+        <f t="shared" ref="AK5" si="20">IF(ISBLANK(W5),IF(ISBLANK(AD5),"",AD5),W5+AD5)</f>
         <v/>
       </c>
-      <c r="AL5" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AM5" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AN5" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AO5" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AP5" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AQ5" s="18">
-        <v>1000</v>
-      </c>
-      <c r="AS5">
-        <v>3</v>
-      </c>
-      <c r="AT5">
-        <f t="shared" ref="AT5:AX5" si="18">AS5+0.1</f>
-        <v>3.1</v>
+      <c r="AN5">
+        <v>21590220</v>
+      </c>
+      <c r="AO5">
+        <v>19892852</v>
+      </c>
+      <c r="AP5">
+        <v>24528246</v>
+      </c>
+      <c r="AQ5" s="20">
+        <v>21996103</v>
+      </c>
+      <c r="AS5" s="21">
+        <v>17912</v>
+      </c>
+      <c r="AT5" s="21">
+        <v>18104</v>
       </c>
       <c r="AU5">
-        <f t="shared" si="18"/>
-        <v>3.2</v>
+        <v>20057</v>
       </c>
       <c r="AV5">
-        <f t="shared" si="18"/>
-        <v>3.3000000000000003</v>
+        <v>20960</v>
       </c>
       <c r="AW5">
-        <f t="shared" si="18"/>
-        <v>3.4000000000000004</v>
-      </c>
-      <c r="AX5">
-        <f t="shared" si="18"/>
-        <v>3.5000000000000004</v>
+        <v>22142</v>
+      </c>
+      <c r="AX5" s="20">
+        <v>22591</v>
       </c>
     </row>
     <row r="6" spans="1:52">
       <c r="A6" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>393</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>399</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>56</v>
@@ -5101,140 +5075,155 @@
       <c r="I6" s="3">
         <v>44561</v>
       </c>
-      <c r="J6" s="22">
-        <v>19310000000</v>
-      </c>
-      <c r="K6" s="22">
-        <v>6974000000</v>
-      </c>
-      <c r="L6" s="22">
-        <v>25930000000</v>
-      </c>
-      <c r="M6" s="22">
-        <f>L6+411000000</f>
-        <v>26341000000</v>
-      </c>
-      <c r="N6" s="22">
-        <v>39504000000</v>
+      <c r="J6">
+        <v>16000</v>
+      </c>
+      <c r="K6">
+        <v>2000</v>
+      </c>
+      <c r="L6">
+        <v>100000</v>
+      </c>
+      <c r="M6">
+        <v>400000</v>
+      </c>
+      <c r="N6">
+        <f>1000000+L6</f>
+        <v>1100000</v>
       </c>
       <c r="O6" t="s">
         <v>58</v>
       </c>
       <c r="P6" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q6" s="20">
-        <v>1040335</v>
-      </c>
-      <c r="R6" s="20">
-        <v>965570</v>
+        <v>402</v>
+      </c>
+      <c r="Q6">
+        <v>1000</v>
+      </c>
+      <c r="R6">
+        <v>995</v>
       </c>
       <c r="S6">
-        <v>1363231</v>
+        <v>990</v>
       </c>
       <c r="T6">
-        <v>1934393</v>
+        <v>985</v>
       </c>
       <c r="U6">
-        <v>1416448</v>
+        <v>980</v>
       </c>
       <c r="V6">
-        <f>1590305</f>
-        <v>1590305</v>
-      </c>
+        <v>975</v>
+      </c>
+      <c r="W6"/>
       <c r="X6">
+        <v>100</v>
+      </c>
+      <c r="Y6">
+        <v>99</v>
+      </c>
+      <c r="Z6">
+        <v>98</v>
+      </c>
+      <c r="AA6">
+        <v>97</v>
+      </c>
+      <c r="AB6">
+        <v>96</v>
+      </c>
+      <c r="AC6">
+        <v>95</v>
+      </c>
+      <c r="AD6" s="18"/>
+      <c r="AE6" s="19">
+        <f t="shared" ref="AE6:AK7" si="21">IF(ISBLANK(Q6),IF(ISBLANK(X6),"",X6),Q6+X6)</f>
+        <v>1100</v>
+      </c>
+      <c r="AF6" s="19">
+        <f t="shared" si="21"/>
+        <v>1094</v>
+      </c>
+      <c r="AG6" s="19">
+        <f t="shared" si="21"/>
+        <v>1088</v>
+      </c>
+      <c r="AH6" s="19">
+        <f t="shared" si="21"/>
+        <v>1082</v>
+      </c>
+      <c r="AI6" s="19">
+        <f t="shared" si="21"/>
+        <v>1076</v>
+      </c>
+      <c r="AJ6" s="19">
+        <f t="shared" si="21"/>
+        <v>1070</v>
+      </c>
+      <c r="AK6" s="19" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AL6" s="18">
         <v>0</v>
       </c>
-      <c r="Y6">
+      <c r="AM6" s="18">
         <v>0</v>
       </c>
-      <c r="Z6">
-        <v>381533</v>
-      </c>
-      <c r="AA6">
-        <v>231192</v>
-      </c>
-      <c r="AB6">
-        <v>297283</v>
-      </c>
-      <c r="AC6" s="20">
-        <v>273432</v>
-      </c>
-      <c r="AE6" s="19">
-        <f t="shared" si="11"/>
-        <v>1040335</v>
-      </c>
-      <c r="AF6" s="19">
-        <f t="shared" si="12"/>
-        <v>965570</v>
-      </c>
-      <c r="AG6" s="19">
-        <f t="shared" si="13"/>
-        <v>1744764</v>
-      </c>
-      <c r="AH6" s="19">
-        <f t="shared" si="14"/>
-        <v>2165585</v>
-      </c>
-      <c r="AI6" s="19">
-        <f t="shared" si="15"/>
-        <v>1713731</v>
-      </c>
-      <c r="AJ6" s="19">
-        <f t="shared" si="16"/>
-        <v>1863737</v>
-      </c>
-      <c r="AK6" s="19" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AN6">
-        <v>21590220</v>
-      </c>
-      <c r="AO6">
-        <v>19892852</v>
-      </c>
-      <c r="AP6">
-        <v>24528246</v>
-      </c>
-      <c r="AQ6" s="20">
-        <v>21996103</v>
-      </c>
-      <c r="AS6" s="21">
-        <v>17912</v>
-      </c>
-      <c r="AT6" s="21">
-        <v>18104</v>
+      <c r="AN6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="18"/>
+      <c r="AS6">
+        <v>3</v>
+      </c>
+      <c r="AT6">
+        <f>AS6+0.1</f>
+        <v>3.1</v>
       </c>
       <c r="AU6">
-        <v>20057</v>
+        <f t="shared" ref="AU6:AX6" si="22">AT6+0.1</f>
+        <v>3.2</v>
       </c>
       <c r="AV6">
-        <v>20960</v>
+        <f t="shared" si="22"/>
+        <v>3.3000000000000003</v>
       </c>
       <c r="AW6">
-        <v>22142</v>
-      </c>
-      <c r="AX6" s="20">
-        <v>22591</v>
-      </c>
+        <f t="shared" si="22"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="AX6">
+        <f t="shared" si="22"/>
+        <v>3.5000000000000004</v>
+      </c>
+      <c r="AY6" s="18"/>
+      <c r="AZ6" s="18"/>
     </row>
     <row r="7" spans="1:52">
       <c r="A7" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>395</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>56</v>
@@ -5245,136 +5234,148 @@
       <c r="I7" s="3">
         <v>44561</v>
       </c>
-      <c r="J7" s="22">
-        <v>19310000000</v>
-      </c>
-      <c r="K7" s="22">
-        <v>6974000000</v>
-      </c>
-      <c r="L7" s="22">
-        <v>25930000000</v>
-      </c>
-      <c r="M7" s="22">
-        <f>L7+411000000</f>
-        <v>26341000000</v>
-      </c>
-      <c r="N7" s="22">
-        <v>39504000000</v>
+      <c r="J7">
+        <v>8000</v>
+      </c>
+      <c r="K7">
+        <v>4000</v>
+      </c>
+      <c r="L7">
+        <v>200000</v>
+      </c>
+      <c r="M7">
+        <v>400000</v>
+      </c>
+      <c r="N7">
+        <f>1000000+L7</f>
+        <v>1200000</v>
       </c>
       <c r="O7" t="s">
         <v>58</v>
       </c>
       <c r="P7" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q7" s="20">
-        <v>1040335</v>
-      </c>
-      <c r="R7" s="20">
-        <v>965570</v>
+        <v>402</v>
+      </c>
+      <c r="Q7">
+        <v>1000</v>
+      </c>
+      <c r="R7">
+        <v>995</v>
       </c>
       <c r="S7">
-        <v>1363231</v>
+        <v>990</v>
       </c>
       <c r="T7">
-        <v>1934393</v>
+        <v>985</v>
       </c>
       <c r="U7">
-        <v>1416448</v>
+        <v>980</v>
       </c>
       <c r="V7">
-        <f>1590305</f>
-        <v>1590305</v>
-      </c>
+        <v>975</v>
+      </c>
+      <c r="W7"/>
       <c r="X7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Y7">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="Z7">
-        <v>381533</v>
+        <v>98</v>
       </c>
       <c r="AA7">
-        <v>231192</v>
+        <v>97</v>
       </c>
       <c r="AB7">
-        <v>297283</v>
-      </c>
-      <c r="AC7" s="20">
-        <v>273432</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="AC7">
+        <v>95</v>
+      </c>
+      <c r="AD7"/>
       <c r="AE7" s="19">
-        <f t="shared" si="11"/>
-        <v>1040335</v>
+        <f t="shared" si="21"/>
+        <v>1100</v>
       </c>
       <c r="AF7" s="19">
-        <f t="shared" si="11"/>
-        <v>965570</v>
+        <f t="shared" si="21"/>
+        <v>1094</v>
       </c>
       <c r="AG7" s="19">
-        <f t="shared" si="11"/>
-        <v>1744764</v>
+        <f t="shared" si="21"/>
+        <v>1088</v>
       </c>
       <c r="AH7" s="19">
-        <f t="shared" si="11"/>
-        <v>2165585</v>
+        <f t="shared" si="21"/>
+        <v>1082</v>
       </c>
       <c r="AI7" s="19">
-        <f t="shared" si="11"/>
-        <v>1713731</v>
+        <f t="shared" si="21"/>
+        <v>1076</v>
       </c>
       <c r="AJ7" s="19">
-        <f t="shared" si="11"/>
-        <v>1863737</v>
+        <f t="shared" si="21"/>
+        <v>1070</v>
       </c>
       <c r="AK7" s="19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="AN7">
-        <v>21590220</v>
-      </c>
-      <c r="AO7">
-        <v>19892852</v>
-      </c>
-      <c r="AP7">
-        <v>24528246</v>
-      </c>
-      <c r="AQ7" s="20">
-        <v>21996103</v>
-      </c>
-      <c r="AS7" s="21">
-        <v>17912</v>
-      </c>
-      <c r="AT7" s="21">
-        <v>18104</v>
+      <c r="AL7" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AM7" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AN7" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AO7" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AP7" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AQ7" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AS7">
+        <v>3</v>
+      </c>
+      <c r="AT7">
+        <f t="shared" ref="AT7:AX7" si="23">AS7+0.1</f>
+        <v>3.1</v>
       </c>
       <c r="AU7">
-        <v>20057</v>
+        <f t="shared" si="23"/>
+        <v>3.2</v>
       </c>
       <c r="AV7">
-        <v>20960</v>
+        <f t="shared" si="23"/>
+        <v>3.3000000000000003</v>
       </c>
       <c r="AW7">
-        <v>22142</v>
-      </c>
-      <c r="AX7" s="20">
-        <v>22591</v>
+        <f t="shared" si="23"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="AX7">
+        <f t="shared" si="23"/>
+        <v>3.5000000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:52">
       <c r="A8" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>401</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" t="s">
@@ -5389,126 +5390,291 @@
       <c r="I8" s="3">
         <v>44561</v>
       </c>
-      <c r="J8" s="22">
-        <v>19310000000</v>
-      </c>
-      <c r="K8" s="22">
-        <v>6974000000</v>
-      </c>
-      <c r="L8" s="22">
-        <v>25930000000</v>
-      </c>
-      <c r="M8" s="22">
-        <f>L8+411000000</f>
-        <v>26341000000</v>
-      </c>
-      <c r="N8" s="22">
-        <v>39504000000</v>
+      <c r="J8">
+        <v>4000</v>
+      </c>
+      <c r="K8">
+        <v>8000</v>
+      </c>
+      <c r="L8">
+        <v>300000</v>
+      </c>
+      <c r="M8">
+        <v>400000</v>
+      </c>
+      <c r="N8">
+        <f>1000000+L8</f>
+        <v>1300000</v>
       </c>
       <c r="O8" t="s">
         <v>58</v>
       </c>
       <c r="P8" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q8" s="20">
-        <v>1040335</v>
-      </c>
-      <c r="R8" s="20">
-        <v>965570</v>
+        <v>402</v>
+      </c>
+      <c r="Q8">
+        <v>1000</v>
+      </c>
+      <c r="R8">
+        <v>995</v>
       </c>
       <c r="S8">
-        <v>1363231</v>
+        <v>990</v>
       </c>
       <c r="T8">
-        <v>1934393</v>
+        <v>985</v>
       </c>
       <c r="U8">
-        <v>1416448</v>
+        <v>980</v>
       </c>
       <c r="V8">
-        <f>1590305</f>
-        <v>1590305</v>
-      </c>
+        <v>975</v>
+      </c>
+      <c r="W8"/>
       <c r="X8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Y8">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="Z8">
-        <v>381533</v>
+        <v>98</v>
       </c>
       <c r="AA8">
-        <v>231192</v>
+        <v>97</v>
       </c>
       <c r="AB8">
-        <v>297283</v>
-      </c>
-      <c r="AC8" s="20">
-        <v>273432</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="AC8">
+        <v>95</v>
+      </c>
+      <c r="AD8"/>
       <c r="AE8" s="19">
-        <f t="shared" ref="AE8" si="19">IF(ISBLANK(Q8),IF(ISBLANK(X8),"",X8),Q8+X8)</f>
-        <v>1040335</v>
+        <f t="shared" ref="AE8" si="24">IF(ISBLANK(Q8),IF(ISBLANK(X8),"",X8),Q8+X8)</f>
+        <v>1100</v>
       </c>
       <c r="AF8" s="19">
-        <f t="shared" ref="AF8" si="20">IF(ISBLANK(R8),IF(ISBLANK(Y8),"",Y8),R8+Y8)</f>
-        <v>965570</v>
+        <f t="shared" ref="AF8" si="25">IF(ISBLANK(R8),IF(ISBLANK(Y8),"",Y8),R8+Y8)</f>
+        <v>1094</v>
       </c>
       <c r="AG8" s="19">
-        <f t="shared" ref="AG8" si="21">IF(ISBLANK(S8),IF(ISBLANK(Z8),"",Z8),S8+Z8)</f>
-        <v>1744764</v>
+        <f t="shared" ref="AG8" si="26">IF(ISBLANK(S8),IF(ISBLANK(Z8),"",Z8),S8+Z8)</f>
+        <v>1088</v>
       </c>
       <c r="AH8" s="19">
-        <f t="shared" ref="AH8" si="22">IF(ISBLANK(T8),IF(ISBLANK(AA8),"",AA8),T8+AA8)</f>
-        <v>2165585</v>
+        <f t="shared" ref="AH8" si="27">IF(ISBLANK(T8),IF(ISBLANK(AA8),"",AA8),T8+AA8)</f>
+        <v>1082</v>
       </c>
       <c r="AI8" s="19">
-        <f t="shared" ref="AI8" si="23">IF(ISBLANK(U8),IF(ISBLANK(AB8),"",AB8),U8+AB8)</f>
-        <v>1713731</v>
+        <f t="shared" ref="AI8" si="28">IF(ISBLANK(U8),IF(ISBLANK(AB8),"",AB8),U8+AB8)</f>
+        <v>1076</v>
       </c>
       <c r="AJ8" s="19">
-        <f t="shared" ref="AJ8" si="24">IF(ISBLANK(V8),IF(ISBLANK(AC8),"",AC8),V8+AC8)</f>
-        <v>1863737</v>
+        <f t="shared" ref="AJ8" si="29">IF(ISBLANK(V8),IF(ISBLANK(AC8),"",AC8),V8+AC8)</f>
+        <v>1070</v>
       </c>
       <c r="AK8" s="19" t="str">
-        <f t="shared" ref="AK8" si="25">IF(ISBLANK(W8),IF(ISBLANK(AD8),"",AD8),W8+AD8)</f>
+        <f t="shared" ref="AK8" si="30">IF(ISBLANK(W8),IF(ISBLANK(AD8),"",AD8),W8+AD8)</f>
         <v/>
       </c>
-      <c r="AN8">
-        <v>21590220</v>
-      </c>
-      <c r="AO8">
-        <v>19892852</v>
-      </c>
-      <c r="AP8">
-        <v>24528246</v>
-      </c>
-      <c r="AQ8" s="20">
-        <v>21996103</v>
-      </c>
-      <c r="AS8" s="21">
-        <v>17912</v>
-      </c>
-      <c r="AT8" s="21">
-        <v>18104</v>
+      <c r="AL8" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AM8" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AN8" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AO8" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AP8" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AQ8" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AS8">
+        <v>3</v>
+      </c>
+      <c r="AT8">
+        <f t="shared" ref="AT8:AX8" si="31">AS8+0.1</f>
+        <v>3.1</v>
       </c>
       <c r="AU8">
-        <v>20057</v>
+        <f t="shared" si="31"/>
+        <v>3.2</v>
       </c>
       <c r="AV8">
-        <v>20960</v>
+        <f t="shared" si="31"/>
+        <v>3.3000000000000003</v>
       </c>
       <c r="AW8">
-        <v>22142</v>
-      </c>
-      <c r="AX8" s="20">
-        <v>22591</v>
+        <f t="shared" si="31"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="AX8">
+        <f t="shared" si="31"/>
+        <v>3.5000000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:52">
-      <c r="E9"/>
+      <c r="A9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" t="s">
+        <v>399</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="3">
+        <v>44561</v>
+      </c>
+      <c r="J9">
+        <v>2000</v>
+      </c>
+      <c r="K9">
+        <v>16000</v>
+      </c>
+      <c r="L9">
+        <v>400000</v>
+      </c>
+      <c r="M9">
+        <v>400000</v>
+      </c>
+      <c r="N9">
+        <f>1000000+L9</f>
+        <v>1400000</v>
+      </c>
+      <c r="O9" t="s">
+        <v>58</v>
+      </c>
+      <c r="P9" t="s">
+        <v>402</v>
+      </c>
+      <c r="Q9">
+        <v>1000</v>
+      </c>
+      <c r="R9">
+        <v>995</v>
+      </c>
+      <c r="S9">
+        <v>990</v>
+      </c>
+      <c r="T9">
+        <v>985</v>
+      </c>
+      <c r="U9">
+        <v>980</v>
+      </c>
+      <c r="V9">
+        <v>975</v>
+      </c>
+      <c r="W9"/>
+      <c r="X9">
+        <v>100</v>
+      </c>
+      <c r="Y9">
+        <v>99</v>
+      </c>
+      <c r="Z9">
+        <v>98</v>
+      </c>
+      <c r="AA9">
+        <v>97</v>
+      </c>
+      <c r="AB9">
+        <v>96</v>
+      </c>
+      <c r="AC9">
+        <v>95</v>
+      </c>
+      <c r="AD9"/>
+      <c r="AE9" s="19">
+        <f>IF(ISBLANK(Q9),IF(ISBLANK(X9),"",X9),Q9+X9)</f>
+        <v>1100</v>
+      </c>
+      <c r="AF9" s="19">
+        <f>IF(ISBLANK(R9),IF(ISBLANK(Y9),"",Y9),R9+Y9)</f>
+        <v>1094</v>
+      </c>
+      <c r="AG9" s="19">
+        <f>IF(ISBLANK(S9),IF(ISBLANK(Z9),"",Z9),S9+Z9)</f>
+        <v>1088</v>
+      </c>
+      <c r="AH9" s="19">
+        <f>IF(ISBLANK(T9),IF(ISBLANK(AA9),"",AA9),T9+AA9)</f>
+        <v>1082</v>
+      </c>
+      <c r="AI9" s="19">
+        <f>IF(ISBLANK(U9),IF(ISBLANK(AB9),"",AB9),U9+AB9)</f>
+        <v>1076</v>
+      </c>
+      <c r="AJ9" s="19">
+        <f>IF(ISBLANK(V9),IF(ISBLANK(AC9),"",AC9),V9+AC9)</f>
+        <v>1070</v>
+      </c>
+      <c r="AK9" s="19" t="str">
+        <f>IF(ISBLANK(W9),IF(ISBLANK(AD9),"",AD9),W9+AD9)</f>
+        <v/>
+      </c>
+      <c r="AL9" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AM9" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AN9" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AO9" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AP9" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AQ9" s="18">
+        <v>1000</v>
+      </c>
+      <c r="AS9">
+        <v>3</v>
+      </c>
+      <c r="AT9">
+        <f t="shared" ref="AT9:AX9" si="32">AS9+0.1</f>
+        <v>3.1</v>
+      </c>
+      <c r="AU9">
+        <f t="shared" si="32"/>
+        <v>3.2</v>
+      </c>
+      <c r="AV9">
+        <f t="shared" si="32"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="AW9">
+        <f t="shared" si="32"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="AX9">
+        <f t="shared" si="32"/>
+        <v>3.5000000000000004</v>
+      </c>
     </row>
     <row r="10" spans="1:52">
       <c r="E10"/>
@@ -14410,13 +14576,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -14477,84 +14643,78 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>388</v>
+        <v>404</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>405</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" t="str">
-        <f>'ITR input data'!D2</f>
-        <v>FR</v>
-      </c>
-      <c r="E2" s="37">
-        <v>2050</v>
-      </c>
-      <c r="F2" s="37" t="s">
+        <v>406</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="28">
+        <v>2040</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>296</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" t="s">
         <v>297</v>
       </c>
-      <c r="H2" s="37">
+      <c r="H2" s="88">
+        <v>2020</v>
+      </c>
+      <c r="I2" s="31">
         <v>2019</v>
       </c>
-      <c r="I2">
-        <v>2016</v>
-      </c>
       <c r="J2" s="38">
-        <f>'ITR input data'!AE2/'ITR input data'!AS2</f>
-        <v>366.66666666666669</v>
-      </c>
-      <c r="K2" s="37" t="str">
-        <f>CONCATENATE('ITR input data'!O2,"/(",'ITR input data'!P2,")")</f>
-        <v>t CO2/(TJ)</v>
-      </c>
-      <c r="L2" s="37">
-        <v>2030</v>
-      </c>
-      <c r="M2" s="39">
-        <v>0.5</v>
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>298</v>
+      </c>
+      <c r="L2">
+        <v>2025</v>
+      </c>
+      <c r="M2" s="40">
+        <v>0.27</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>405</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" t="str">
-        <f>'ITR input data'!D3</f>
-        <v>FR</v>
-      </c>
-      <c r="E3" s="37">
-        <v>2050</v>
-      </c>
-      <c r="F3" s="37" t="s">
+        <v>406</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="28">
+        <v>2040</v>
+      </c>
+      <c r="F3" s="28" t="s">
         <v>296</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" t="s">
         <v>297</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="88">
+        <v>2020</v>
+      </c>
+      <c r="I3" s="31">
         <v>2019</v>
       </c>
-      <c r="I3">
-        <v>2016</v>
-      </c>
       <c r="J3" s="38">
-        <f>'ITR input data'!AE3/'ITR input data'!AS3</f>
-        <v>366.66666666666669</v>
-      </c>
-      <c r="K3" s="37" t="str">
-        <f>CONCATENATE('ITR input data'!O3,"/(",'ITR input data'!P3,")")</f>
-        <v>t CO2/(TJ)</v>
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="K3" s="37" t="s">
+        <v>298</v>
       </c>
       <c r="L3">
         <v>2030</v>
@@ -14564,390 +14724,519 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="28" t="s">
-        <v>390</v>
+      <c r="A4" t="s">
+        <v>404</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="28" t="str">
-        <f>'ITR input data'!D4</f>
-        <v>FR</v>
-      </c>
-      <c r="E4" s="88">
-        <v>2050</v>
-      </c>
-      <c r="F4" s="88" t="s">
+        <v>405</v>
+      </c>
+      <c r="C4" t="s">
+        <v>406</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="28">
+        <v>2040</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>296</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" t="s">
         <v>297</v>
       </c>
       <c r="H4" s="88">
+        <v>2020</v>
+      </c>
+      <c r="I4" s="31">
         <v>2019</v>
       </c>
-      <c r="I4" s="88">
-        <v>2016</v>
-      </c>
-      <c r="J4" s="89">
-        <f>'ITR input data'!AE4/'ITR input data'!AS4</f>
-        <v>366.66666666666669</v>
-      </c>
-      <c r="K4" s="37" t="str">
-        <f>CONCATENATE('ITR input data'!O4,"/(",'ITR input data'!P4,")")</f>
-        <v>t CO2/(TJ)</v>
-      </c>
-      <c r="L4" s="88">
-        <v>2030</v>
-      </c>
-      <c r="M4" s="90">
-        <v>0.5</v>
+      <c r="J4" s="38">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="K4" s="37" t="s">
+        <v>298</v>
+      </c>
+      <c r="L4">
+        <v>2040</v>
+      </c>
+      <c r="M4" s="40">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="28" t="s">
-        <v>391</v>
+      <c r="A5" t="s">
+        <v>397</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="28" t="str">
-        <f>'ITR input data'!D5</f>
-        <v>FR</v>
-      </c>
-      <c r="E5" s="88">
-        <v>2050</v>
-      </c>
-      <c r="F5" s="88" t="s">
-        <v>296</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>297</v>
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>393</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="28">
+        <v>2035</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="G5" t="s">
+        <v>302</v>
       </c>
       <c r="H5" s="88">
-        <v>2019</v>
-      </c>
-      <c r="I5" s="88">
-        <v>2016</v>
-      </c>
-      <c r="J5" s="89">
-        <f>'ITR input data'!AE5/'ITR input data'!AS5</f>
-        <v>366.66666666666669</v>
-      </c>
-      <c r="K5" s="37" t="str">
-        <f>CONCATENATE('ITR input data'!O5,"/(",'ITR input data'!P5,")")</f>
-        <v>t CO2/(TJ)</v>
-      </c>
-      <c r="L5" s="88">
-        <v>2030</v>
-      </c>
-      <c r="M5" s="90">
-        <v>0.5</v>
+        <v>2021</v>
+      </c>
+      <c r="I5" s="31">
+        <v>2015</v>
+      </c>
+      <c r="J5" s="38">
+        <v>1</v>
+      </c>
+      <c r="K5" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="L5">
+        <v>2025</v>
+      </c>
+      <c r="M5" s="40">
+        <v>0.35</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" t="str">
-        <f>'ITR input data'!D2</f>
-        <v>FR</v>
-      </c>
-      <c r="E6" s="88">
-        <v>2050</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>296</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>303</v>
-      </c>
-      <c r="H6" s="37">
-        <v>2019</v>
-      </c>
-      <c r="I6">
-        <v>2016</v>
+        <v>395</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="28">
+        <v>2035</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="G6" t="s">
+        <v>302</v>
+      </c>
+      <c r="H6" s="88">
+        <v>2021</v>
+      </c>
+      <c r="I6" s="31">
+        <v>2015</v>
       </c>
       <c r="J6" s="38">
-        <f>'ITR input data'!AL2/'ITR input data'!AS2</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="37" t="str">
-        <f>CONCATENATE('ITR input data'!O2,"/(",'ITR input data'!P2,")")</f>
-        <v>t CO2/(TJ)</v>
-      </c>
-      <c r="L6" s="37">
-        <v>2030</v>
-      </c>
-      <c r="M6" s="39">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K6" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="L6">
+        <v>2025</v>
+      </c>
+      <c r="M6" s="40">
+        <v>0.35</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
+        <v>400</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>401</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="28">
+        <v>2035</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="G7" t="s">
+        <v>302</v>
+      </c>
+      <c r="H7" s="88">
+        <v>2021</v>
+      </c>
+      <c r="I7" s="31">
+        <v>2015</v>
+      </c>
+      <c r="J7" s="38">
+        <v>1</v>
+      </c>
+      <c r="K7" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7">
+        <v>2025</v>
+      </c>
+      <c r="M7" s="40">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>388</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="str">
+        <f>'ITR input data'!D6</f>
+        <v>FR</v>
+      </c>
+      <c r="E8" s="37">
+        <v>2050</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>296</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>297</v>
+      </c>
+      <c r="H8" s="37">
+        <v>2019</v>
+      </c>
+      <c r="I8">
+        <v>2016</v>
+      </c>
+      <c r="J8" s="38">
+        <f>'ITR input data'!AE6/'ITR input data'!AS6</f>
+        <v>366.66666666666669</v>
+      </c>
+      <c r="K8" s="37" t="str">
+        <f>CONCATENATE('ITR input data'!O6,"/(",'ITR input data'!P6,")")</f>
+        <v>t CO2/(TJ)</v>
+      </c>
+      <c r="L8" s="37">
+        <v>2030</v>
+      </c>
+      <c r="M8" s="39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
         <v>389</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>62</v>
       </c>
-      <c r="D7" t="str">
-        <f>'ITR input data'!D3</f>
+      <c r="D9" t="str">
+        <f>'ITR input data'!D7</f>
         <v>FR</v>
       </c>
-      <c r="E7" s="88">
+      <c r="E9" s="37">
         <v>2050</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F9" s="37" t="s">
         <v>296</v>
       </c>
-      <c r="G7" s="37" t="s">
-        <v>303</v>
-      </c>
-      <c r="H7" s="37">
+      <c r="G9" s="37" t="s">
+        <v>297</v>
+      </c>
+      <c r="H9" s="37">
         <v>2019</v>
       </c>
-      <c r="I7">
+      <c r="I9">
         <v>2016</v>
       </c>
-      <c r="J7" s="38">
-        <f>'ITR input data'!AL3/'ITR input data'!AS3</f>
-        <v>333.33333333333331</v>
-      </c>
-      <c r="K7" s="37" t="str">
-        <f>CONCATENATE('ITR input data'!O3,"/(",'ITR input data'!P3,")")</f>
+      <c r="J9" s="38">
+        <f>'ITR input data'!AE7/'ITR input data'!AS7</f>
+        <v>366.66666666666669</v>
+      </c>
+      <c r="K9" s="37" t="str">
+        <f>CONCATENATE('ITR input data'!O7,"/(",'ITR input data'!P7,")")</f>
         <v>t CO2/(TJ)</v>
       </c>
-      <c r="L7">
+      <c r="L9">
         <v>2030</v>
       </c>
-      <c r="M7" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="28" t="s">
+      <c r="M9" s="40">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="28" t="s">
         <v>390</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C10" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="D8" t="str">
-        <f>'ITR input data'!D4</f>
+      <c r="D10" s="28" t="str">
+        <f>'ITR input data'!D8</f>
         <v>FR</v>
       </c>
-      <c r="E8" s="88">
+      <c r="E10" s="88">
         <v>2050</v>
       </c>
-      <c r="F8" s="88" t="s">
+      <c r="F10" s="88" t="s">
         <v>296</v>
       </c>
-      <c r="G8" s="37" t="s">
-        <v>303</v>
-      </c>
-      <c r="H8" s="88">
+      <c r="G10" s="37" t="s">
+        <v>297</v>
+      </c>
+      <c r="H10" s="88">
         <v>2019</v>
       </c>
-      <c r="I8" s="88">
+      <c r="I10" s="88">
         <v>2016</v>
       </c>
-      <c r="J8" s="38">
-        <f>'ITR input data'!AL4/'ITR input data'!AS4</f>
-        <v>333.33333333333331</v>
-      </c>
-      <c r="K8" s="37" t="str">
-        <f>CONCATENATE('ITR input data'!O4,"/(",'ITR input data'!P4,")")</f>
+      <c r="J10" s="89">
+        <f>'ITR input data'!AE8/'ITR input data'!AS8</f>
+        <v>366.66666666666669</v>
+      </c>
+      <c r="K10" s="37" t="str">
+        <f>CONCATENATE('ITR input data'!O8,"/(",'ITR input data'!P8,")")</f>
         <v>t CO2/(TJ)</v>
       </c>
-      <c r="L8" s="88">
+      <c r="L10" s="88">
         <v>2030</v>
       </c>
-      <c r="M8" s="90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="28" t="s">
+      <c r="M10" s="90">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="28" t="s">
         <v>391</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C11" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D9" t="str">
-        <f>'ITR input data'!D5</f>
+      <c r="D11" s="28" t="str">
+        <f>'ITR input data'!D9</f>
         <v>FR</v>
       </c>
-      <c r="E9" s="88">
+      <c r="E11" s="88">
         <v>2050</v>
       </c>
-      <c r="F9" s="88" t="s">
+      <c r="F11" s="88" t="s">
         <v>296</v>
       </c>
-      <c r="G9" s="37" t="s">
-        <v>303</v>
-      </c>
-      <c r="H9" s="88">
+      <c r="G11" s="37" t="s">
+        <v>297</v>
+      </c>
+      <c r="H11" s="88">
         <v>2019</v>
       </c>
-      <c r="I9" s="88">
+      <c r="I11" s="88">
         <v>2016</v>
       </c>
-      <c r="J9" s="38">
-        <f>'ITR input data'!AL5/'ITR input data'!AS5</f>
-        <v>333.33333333333331</v>
-      </c>
-      <c r="K9" s="37" t="str">
-        <f>CONCATENATE('ITR input data'!O5,"/(",'ITR input data'!P5,")")</f>
+      <c r="J11" s="89">
+        <f>'ITR input data'!AE9/'ITR input data'!AS9</f>
+        <v>366.66666666666669</v>
+      </c>
+      <c r="K11" s="37" t="str">
+        <f>CONCATENATE('ITR input data'!O9,"/(",'ITR input data'!P9,")")</f>
         <v>t CO2/(TJ)</v>
       </c>
-      <c r="L9" s="88">
+      <c r="L11" s="88">
         <v>2030</v>
       </c>
-      <c r="M9" s="90">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" t="s">
-        <v>397</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" t="s">
-        <v>393</v>
-      </c>
-      <c r="D10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="28">
-        <v>2035</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="G10" t="s">
-        <v>302</v>
-      </c>
-      <c r="H10" s="88">
-        <v>2021</v>
-      </c>
-      <c r="I10" s="31">
-        <v>2015</v>
-      </c>
-      <c r="J10" s="38">
-        <v>1</v>
-      </c>
-      <c r="K10" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="L10">
-        <v>2025</v>
-      </c>
-      <c r="M10" s="40">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" t="s">
-        <v>398</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" t="s">
-        <v>395</v>
-      </c>
-      <c r="D11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="28">
-        <v>2035</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="G11" t="s">
-        <v>302</v>
-      </c>
-      <c r="H11" s="88">
-        <v>2021</v>
-      </c>
-      <c r="I11" s="31">
-        <v>2015</v>
-      </c>
-      <c r="J11" s="38">
-        <v>1</v>
-      </c>
-      <c r="K11" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="L11">
-        <v>2025</v>
-      </c>
-      <c r="M11" s="40">
-        <v>0.35</v>
+      <c r="M11" s="90">
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>401</v>
-      </c>
-      <c r="D12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="28">
-        <v>2035</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="G12" t="s">
-        <v>302</v>
-      </c>
-      <c r="H12" s="88">
-        <v>2021</v>
-      </c>
-      <c r="I12" s="31">
-        <v>2015</v>
+        <v>53</v>
+      </c>
+      <c r="D12" t="str">
+        <f>'ITR input data'!D6</f>
+        <v>FR</v>
+      </c>
+      <c r="E12" s="88">
+        <v>2050</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>296</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>303</v>
+      </c>
+      <c r="H12" s="37">
+        <v>2019</v>
+      </c>
+      <c r="I12">
+        <v>2016</v>
       </c>
       <c r="J12" s="38">
+        <f>'ITR input data'!AL6/'ITR input data'!AS6</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="37" t="str">
+        <f>CONCATENATE('ITR input data'!O6,"/(",'ITR input data'!P6,")")</f>
+        <v>t CO2/(TJ)</v>
+      </c>
+      <c r="L12" s="37">
+        <v>2030</v>
+      </c>
+      <c r="M12" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>389</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" t="str">
+        <f>'ITR input data'!D7</f>
+        <v>FR</v>
+      </c>
+      <c r="E13" s="88">
+        <v>2050</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>296</v>
+      </c>
+      <c r="G13" s="37" t="s">
+        <v>303</v>
+      </c>
+      <c r="H13" s="37">
+        <v>2019</v>
+      </c>
+      <c r="I13">
+        <v>2016</v>
+      </c>
+      <c r="J13" s="38">
+        <f>'ITR input data'!AL7/'ITR input data'!AS7</f>
+        <v>333.33333333333331</v>
+      </c>
+      <c r="K13" s="37" t="str">
+        <f>CONCATENATE('ITR input data'!O7,"/(",'ITR input data'!P7,")")</f>
+        <v>t CO2/(TJ)</v>
+      </c>
+      <c r="L13">
+        <v>2030</v>
+      </c>
+      <c r="M13" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="28" t="s">
+        <v>390</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="str">
+        <f>'ITR input data'!D8</f>
+        <v>FR</v>
+      </c>
+      <c r="E14" s="88">
+        <v>2050</v>
+      </c>
+      <c r="F14" s="88" t="s">
+        <v>296</v>
+      </c>
+      <c r="G14" s="37" t="s">
+        <v>303</v>
+      </c>
+      <c r="H14" s="88">
+        <v>2019</v>
+      </c>
+      <c r="I14" s="88">
+        <v>2016</v>
+      </c>
+      <c r="J14" s="38">
+        <f>'ITR input data'!AL8/'ITR input data'!AS8</f>
+        <v>333.33333333333331</v>
+      </c>
+      <c r="K14" s="37" t="str">
+        <f>CONCATENATE('ITR input data'!O8,"/(",'ITR input data'!P8,")")</f>
+        <v>t CO2/(TJ)</v>
+      </c>
+      <c r="L14" s="88">
+        <v>2030</v>
+      </c>
+      <c r="M14" s="90">
         <v>1</v>
       </c>
-      <c r="K12" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="L12">
-        <v>2025</v>
-      </c>
-      <c r="M12" s="40">
-        <v>0.35</v>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="28" t="s">
+        <v>391</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" t="str">
+        <f>'ITR input data'!D9</f>
+        <v>FR</v>
+      </c>
+      <c r="E15" s="88">
+        <v>2050</v>
+      </c>
+      <c r="F15" s="88" t="s">
+        <v>296</v>
+      </c>
+      <c r="G15" s="37" t="s">
+        <v>303</v>
+      </c>
+      <c r="H15" s="88">
+        <v>2019</v>
+      </c>
+      <c r="I15" s="88">
+        <v>2016</v>
+      </c>
+      <c r="J15" s="38">
+        <f>'ITR input data'!AL9/'ITR input data'!AS9</f>
+        <v>333.33333333333331</v>
+      </c>
+      <c r="K15" s="37" t="str">
+        <f>CONCATENATE('ITR input data'!O9,"/(",'ITR input data'!P9,")")</f>
+        <v>t CO2/(TJ)</v>
+      </c>
+      <c r="L15" s="88">
+        <v>2030</v>
+      </c>
+      <c r="M15" s="90">
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -19779,10 +20068,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
@@ -19811,128 +20100,138 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>388</v>
+        <v>404</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>405</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>406</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>406</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E5" ca="1" si="0">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>70701760</v>
+        <v>180195822</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>393</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="E3">
-        <f t="shared" ca="1" si="0"/>
-        <v>138413468</v>
+        <v>74529651</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>395</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E4">
-        <f t="shared" ca="1" si="0"/>
-        <v>238751118</v>
+        <v>64714707</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>391</v>
-      </c>
-      <c r="B5" s="87" t="s">
-        <v>73</v>
+        <v>400</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>401</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E5">
-        <f t="shared" ca="1" si="0"/>
-        <v>186474255</v>
+        <v>71049976</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>393</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E8" ca="1" si="1">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>262261935</v>
+        <v>123771318</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>395</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E7">
-        <f t="shared" ca="1" si="1"/>
-        <v>99986250</v>
+        <v>85519434</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>401</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E8">
-        <f t="shared" ca="1" si="1"/>
-        <v>266192015</v>
+        <v>57784860</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B9" s="87" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9">
+        <v>230353227</v>
       </c>
     </row>
   </sheetData>
@@ -19991,7 +20290,7 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E66" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
-        <v>214215</v>
+        <v>249578</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -20009,7 +20308,7 @@
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>165514</v>
+        <v>205413</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -20027,7 +20326,7 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>107554</v>
+        <v>114019</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -20045,7 +20344,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>46216</v>
+        <v>241150</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -20063,7 +20362,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>154361</v>
+        <v>123020</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -20081,7 +20380,7 @@
       </c>
       <c r="E7">
         <f t="shared" ref="E7:E8" ca="1" si="1">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>220891902</v>
+        <v>213528336</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -20099,7 +20398,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>141074768</v>
+        <v>50258151</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -20117,7 +20416,7 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>67694</v>
+        <v>151979</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -20135,7 +20434,7 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>40887</v>
+        <v>227471</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -20153,7 +20452,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>38774</v>
+        <v>179511</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -20171,7 +20470,7 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>97706</v>
+        <v>128677</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -20189,7 +20488,7 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>247128</v>
+        <v>214665</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -20207,7 +20506,7 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>68910</v>
+        <v>49902</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -20225,7 +20524,7 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>95947</v>
+        <v>61267</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -20243,7 +20542,7 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>167755</v>
+        <v>185147</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -20261,7 +20560,7 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>198420</v>
+        <v>196431</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -20279,7 +20578,7 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>128406</v>
+        <v>41585</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -20297,7 +20596,7 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>56278</v>
+        <v>132548</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -20315,7 +20614,7 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>229029</v>
+        <v>73156</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -20333,7 +20632,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>113560</v>
+        <v>45981</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -20351,7 +20650,7 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>227073</v>
+        <v>228486</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -20369,7 +20668,7 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>80466</v>
+        <v>43733</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -20387,7 +20686,7 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>77911</v>
+        <v>175041</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -20405,7 +20704,7 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>49038</v>
+        <v>135723</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -20423,7 +20722,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
-        <v>59055</v>
+        <v>81471</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -20441,7 +20740,7 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>52239</v>
+        <v>40464</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -20459,7 +20758,7 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>231630</v>
+        <v>70145</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -20477,7 +20776,7 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
-        <v>90621</v>
+        <v>223034</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -20495,7 +20794,7 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>99898</v>
+        <v>128906</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -20513,7 +20812,7 @@
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>45724</v>
+        <v>214537</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -20531,7 +20830,7 @@
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="0"/>
-        <v>191269</v>
+        <v>186795</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -20549,7 +20848,7 @@
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="0"/>
-        <v>239097</v>
+        <v>227107</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -20567,7 +20866,7 @@
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="0"/>
-        <v>70666</v>
+        <v>143147</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -20585,7 +20884,7 @@
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="0"/>
-        <v>219368</v>
+        <v>62655</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -20603,7 +20902,7 @@
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="0"/>
-        <v>72898</v>
+        <v>172391</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -20621,7 +20920,7 @@
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="0"/>
-        <v>163044</v>
+        <v>94767</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -20639,7 +20938,7 @@
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="0"/>
-        <v>44837</v>
+        <v>57516</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -20657,7 +20956,7 @@
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="0"/>
-        <v>130192</v>
+        <v>102638</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -20675,7 +20974,7 @@
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="0"/>
-        <v>215161</v>
+        <v>96535</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -20693,7 +20992,7 @@
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="0"/>
-        <v>61633</v>
+        <v>225960</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -20711,7 +21010,7 @@
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="0"/>
-        <v>64291</v>
+        <v>39635</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -20729,7 +21028,7 @@
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="0"/>
-        <v>76084</v>
+        <v>106206</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -20747,7 +21046,7 @@
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="0"/>
-        <v>209546</v>
+        <v>65009</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -20765,7 +21064,7 @@
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="0"/>
-        <v>87557</v>
+        <v>93291</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -20783,7 +21082,7 @@
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="0"/>
-        <v>124387</v>
+        <v>132819</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -20801,7 +21100,7 @@
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="0"/>
-        <v>100117</v>
+        <v>201142</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -20819,7 +21118,7 @@
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="0"/>
-        <v>63990</v>
+        <v>243373</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -20837,7 +21136,7 @@
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="0"/>
-        <v>204422</v>
+        <v>167251</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -20855,7 +21154,7 @@
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="0"/>
-        <v>156380</v>
+        <v>87340</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -20873,7 +21172,7 @@
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="0"/>
-        <v>113292</v>
+        <v>112570</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -20891,7 +21190,7 @@
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="0"/>
-        <v>234411</v>
+        <v>243511</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -20909,7 +21208,7 @@
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="0"/>
-        <v>181340</v>
+        <v>55204</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -20927,7 +21226,7 @@
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="0"/>
-        <v>91265</v>
+        <v>37888</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -20945,7 +21244,7 @@
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="0"/>
-        <v>82305</v>
+        <v>202879</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -20963,7 +21262,7 @@
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="0"/>
-        <v>90090</v>
+        <v>89336</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -20981,7 +21280,7 @@
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="0"/>
-        <v>85115</v>
+        <v>142170</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -20999,7 +21298,7 @@
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="0"/>
-        <v>74086</v>
+        <v>71004</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -21017,7 +21316,7 @@
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="0"/>
-        <v>75243</v>
+        <v>186674</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -21035,7 +21334,7 @@
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="0"/>
-        <v>53512</v>
+        <v>201994</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -21053,7 +21352,7 @@
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="0"/>
-        <v>159611</v>
+        <v>240344</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -21071,7 +21370,7 @@
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="0"/>
-        <v>208356</v>
+        <v>232278</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -21089,7 +21388,7 @@
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="0"/>
-        <v>173592</v>
+        <v>111569</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -21107,7 +21406,7 @@
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="0"/>
-        <v>95987</v>
+        <v>99394</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -21125,7 +21424,7 @@
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="0"/>
-        <v>130862</v>
+        <v>46687</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -21143,7 +21442,7 @@
       </c>
       <c r="E66">
         <f t="shared" ca="1" si="0"/>
-        <v>184312</v>
+        <v>61587</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -21161,7 +21460,7 @@
       </c>
       <c r="E67">
         <f t="shared" ref="E67:E69" ca="1" si="2">RANDBETWEEN(35000,250000)</f>
-        <v>114153</v>
+        <v>40720</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -21179,7 +21478,7 @@
       </c>
       <c r="E68">
         <f t="shared" ca="1" si="2"/>
-        <v>41173</v>
+        <v>143047</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -21197,7 +21496,7 @@
       </c>
       <c r="E69">
         <f t="shared" ca="1" si="2"/>
-        <v>65959</v>
+        <v>214518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>